<commit_message>
raw sorded visualisations CZtransl+barplots
</commit_message>
<xml_diff>
--- a/qualityoflife_sourcedesc.xlsx
+++ b/qualityoflife_sourcedesc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarogumulec/Documents/Kody/QualityOfLife/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB99AAB7-CC7C-144F-BAEC-8ADF779E6DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F5AA69-BB2A-5148-8427-78C16FE71EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{72E829D7-3EE3-4F5A-80DA-9E2BC7D33FF7}"/>
   </bookViews>
@@ -2689,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC34AECA-0233-8F4D-9A6A-7C98DF6640BF}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="143" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3809,7 +3809,7 @@
       <c r="G43" t="s">
         <v>730</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="6" t="s">
         <v>731</v>
       </c>
       <c r="I43" t="s">
@@ -3846,6 +3846,7 @@
     <hyperlink ref="H20" r:id="rId3" xr:uid="{1C547B13-CEA9-3A49-95C9-D3DD5AFF9DF4}"/>
     <hyperlink ref="H21" r:id="rId4" xr:uid="{E8A16D9B-5F27-ED41-89AB-193AF8C0B0F0}"/>
     <hyperlink ref="H22" r:id="rId5" xr:uid="{9FCC0F3E-9A61-FF43-A4A2-857CEC99F442}"/>
+    <hyperlink ref="H43" r:id="rId6" xr:uid="{801CE65E-5FA0-604B-B6A0-3CA4791D9CFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>